<commit_message>
Open on correct page
</commit_message>
<xml_diff>
--- a/CompLaagBond/files/template-excel-bk-indoor-indiv.xlsx
+++ b/CompLaagBond/files/template-excel-bk-indoor-indiv.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projects Ramon\Websites\NHB-applicaties\Excel programma's\BK excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3527F02-C474-41BC-8E6D-592AE6ED9A99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1BD63F3-571A-4FD7-8D53-CD72853A5D57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1770" yWindow="1320" windowWidth="22440" windowHeight="14040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6045" yWindow="1410" windowWidth="22440" windowHeight="14040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Uitleg" sheetId="3" r:id="rId1"/>
@@ -1383,7 +1383,7 @@
   <sheetPr codeName="Blad5"/>
   <dimension ref="A1:B52"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1693,7 +1693,7 @@
   </sheetPr>
   <dimension ref="A1:W38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>

<commit_message>
Repaired transport formulas in BK individual program
</commit_message>
<xml_diff>
--- a/CompLaagBond/files/template-excel-bk-indoor-indiv.xlsx
+++ b/CompLaagBond/files/template-excel-bk-indoor-indiv.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projects Ramon\Websites\NHB-applicaties\Excel programma's\BK excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65D37EFA-C680-4199-AACE-B6A7EBF14042}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B78C9B9-07A2-4079-8031-D181D3DA6EF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2115" yWindow="1410" windowWidth="18195" windowHeight="14025" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10605" yWindow="645" windowWidth="18195" windowHeight="14025" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Uitleg" sheetId="3" r:id="rId1"/>
@@ -2824,8 +2824,8 @@
   </sheetPr>
   <dimension ref="A1:L97"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:L1"/>
+    <sheetView topLeftCell="A27" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.25" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
@@ -3706,7 +3706,7 @@
     </row>
     <row r="64" spans="1:12" s="27" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="B64" s="47" t="str">
-        <f>IF(Voorronde!N9&gt;0,"["&amp;Voorronde!D9&amp;"] "&amp;Voorronde!E38,"BYE")</f>
+        <f>IF(Voorronde!N9&gt;0,"["&amp;Voorronde!D9&amp;"] "&amp;Voorronde!E9,"BYE")</f>
         <v>BYE</v>
       </c>
       <c r="H64" s="48" t="str">
@@ -3716,7 +3716,7 @@
     </row>
     <row r="65" spans="2:8" s="27" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="B65" s="47" t="str">
-        <f>IF(Voorronde!N10&gt;0,"["&amp;Voorronde!D10&amp;"] "&amp;Voorronde!E39,"BYE")</f>
+        <f>IF(Voorronde!N10&gt;0,"["&amp;Voorronde!D10&amp;"] "&amp;Voorronde!E10,"BYE")</f>
         <v>BYE</v>
       </c>
       <c r="H65" s="48" t="str">
@@ -3726,7 +3726,7 @@
     </row>
     <row r="66" spans="2:8" s="27" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="B66" s="47" t="str">
-        <f>IF(Voorronde!N11&gt;0,"["&amp;Voorronde!D11&amp;"] "&amp;Voorronde!E40,"BYE")</f>
+        <f>IF(Voorronde!N11&gt;0,"["&amp;Voorronde!D11&amp;"] "&amp;Voorronde!E11,"BYE")</f>
         <v>BYE</v>
       </c>
       <c r="H66" s="48" t="str">
@@ -3736,7 +3736,7 @@
     </row>
     <row r="67" spans="2:8" s="27" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="B67" s="47" t="str">
-        <f>IF(Voorronde!N12&gt;0,"["&amp;Voorronde!D12&amp;"] "&amp;Voorronde!E41,"BYE")</f>
+        <f>IF(Voorronde!N12&gt;0,"["&amp;Voorronde!D12&amp;"] "&amp;Voorronde!E12,"BYE")</f>
         <v>BYE</v>
       </c>
       <c r="H67" s="27" t="str">
@@ -3865,8 +3865,8 @@
   </sheetPr>
   <dimension ref="A1:X97"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:R1"/>
+    <sheetView topLeftCell="A33" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A52" sqref="A52:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.25" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
@@ -5051,7 +5051,7 @@
       <c r="Q51" s="27"/>
       <c r="R51" s="27"/>
     </row>
-    <row r="52" spans="1:18" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:18" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52" s="29"/>
       <c r="B52" s="27"/>
       <c r="C52" s="27"/>
@@ -5151,7 +5151,7 @@
     </row>
     <row r="64" spans="1:18" s="27" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="B64" s="47" t="str">
-        <f>IF(Voorronde!N9&gt;0,"["&amp;Voorronde!D9&amp;"] "&amp;Voorronde!E38,"BYE")</f>
+        <f>IF(Voorronde!N9&gt;0,"["&amp;Voorronde!D9&amp;"] "&amp;Voorronde!E9,"BYE")</f>
         <v>BYE</v>
       </c>
       <c r="H64" s="48" t="str">
@@ -5165,7 +5165,7 @@
     </row>
     <row r="65" spans="2:14" s="27" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="B65" s="47" t="str">
-        <f>IF(Voorronde!N10&gt;0,"["&amp;Voorronde!D10&amp;"] "&amp;Voorronde!E39,"BYE")</f>
+        <f>IF(Voorronde!N10&gt;0,"["&amp;Voorronde!D10&amp;"] "&amp;Voorronde!E10,"BYE")</f>
         <v>BYE</v>
       </c>
       <c r="H65" s="48" t="str">
@@ -5179,7 +5179,7 @@
     </row>
     <row r="66" spans="2:14" s="27" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="B66" s="47" t="str">
-        <f>IF(Voorronde!N11&gt;0,"["&amp;Voorronde!D11&amp;"] "&amp;Voorronde!E40,"BYE")</f>
+        <f>IF(Voorronde!N11&gt;0,"["&amp;Voorronde!D11&amp;"] "&amp;Voorronde!E11,"BYE")</f>
         <v>BYE</v>
       </c>
       <c r="H66" s="48" t="str">
@@ -5193,7 +5193,7 @@
     </row>
     <row r="67" spans="2:14" s="27" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="B67" s="47" t="str">
-        <f>IF(Voorronde!N12&gt;0,"["&amp;Voorronde!D12&amp;"] "&amp;Voorronde!E41,"BYE")</f>
+        <f>IF(Voorronde!N12&gt;0,"["&amp;Voorronde!D12&amp;"] "&amp;Voorronde!E12,"BYE")</f>
         <v>BYE</v>
       </c>
       <c r="H67" s="48" t="str">
@@ -5207,25 +5207,25 @@
     </row>
     <row r="68" spans="2:14" s="27" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="B68" s="47" t="str">
-        <f>IF(Voorronde!N13&gt;0,"["&amp;Voorronde!D13&amp;"] "&amp;Voorronde!E42,"BYE")</f>
+        <f>IF(Voorronde!N13&gt;0,"["&amp;Voorronde!D13&amp;"] "&amp;Voorronde!E13,"BYE")</f>
         <v>BYE</v>
       </c>
     </row>
     <row r="69" spans="2:14" s="27" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="B69" s="47" t="str">
-        <f>IF(Voorronde!N14&gt;0,"["&amp;Voorronde!D14&amp;"] "&amp;Voorronde!E43,"BYE")</f>
+        <f>IF(Voorronde!N14&gt;0,"["&amp;Voorronde!D14&amp;"] "&amp;Voorronde!E14,"BYE")</f>
         <v>BYE</v>
       </c>
     </row>
     <row r="70" spans="2:14" s="27" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="B70" s="47" t="str">
-        <f>IF(Voorronde!N15&gt;0,"["&amp;Voorronde!D15&amp;"] "&amp;Voorronde!E44,"BYE")</f>
+        <f>IF(Voorronde!N15&gt;0,"["&amp;Voorronde!D15&amp;"] "&amp;Voorronde!E15,"BYE")</f>
         <v>BYE</v>
       </c>
     </row>
     <row r="71" spans="2:14" s="27" customFormat="1" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="B71" s="47" t="str">
-        <f>IF(Voorronde!N16&gt;0,"["&amp;Voorronde!D16&amp;"] "&amp;Voorronde!E45,"BYE")</f>
+        <f>IF(Voorronde!N16&gt;0,"["&amp;Voorronde!D16&amp;"] "&amp;Voorronde!E16,"BYE")</f>
         <v>BYE</v>
       </c>
     </row>
@@ -7172,7 +7172,7 @@
     <row r="64" spans="1:24" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" s="30"/>
       <c r="B64" s="47" t="str">
-        <f>IF(Voorronde!N9&gt;0,"["&amp;Voorronde!D9&amp;"] "&amp;Voorronde!E38,"BYE")</f>
+        <f>IF(Voorronde!N9&gt;0,"["&amp;Voorronde!D9&amp;"] "&amp;Voorronde!E9,"BYE")</f>
         <v>BYE</v>
       </c>
       <c r="C64" s="29"/>
@@ -7194,7 +7194,7 @@
     <row r="65" spans="1:20" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65" s="30"/>
       <c r="B65" s="47" t="str">
-        <f>IF(Voorronde!N10&gt;0,"["&amp;Voorronde!D10&amp;"] "&amp;Voorronde!E39,"BYE")</f>
+        <f>IF(Voorronde!N10&gt;0,"["&amp;Voorronde!D10&amp;"] "&amp;Voorronde!E10,"BYE")</f>
         <v>BYE</v>
       </c>
       <c r="C65" s="29"/>
@@ -7216,7 +7216,7 @@
     <row r="66" spans="1:20" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66" s="30"/>
       <c r="B66" s="47" t="str">
-        <f>IF(Voorronde!N11&gt;0,"["&amp;Voorronde!D11&amp;"] "&amp;Voorronde!E40,"BYE")</f>
+        <f>IF(Voorronde!N11&gt;0,"["&amp;Voorronde!D11&amp;"] "&amp;Voorronde!E11,"BYE")</f>
         <v>BYE</v>
       </c>
       <c r="C66" s="29"/>
@@ -7238,7 +7238,7 @@
     <row r="67" spans="1:20" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67" s="30"/>
       <c r="B67" s="47" t="str">
-        <f>IF(Voorronde!N12&gt;0,"["&amp;Voorronde!D12&amp;"] "&amp;Voorronde!E41,"BYE")</f>
+        <f>IF(Voorronde!N12&gt;0,"["&amp;Voorronde!D12&amp;"] "&amp;Voorronde!E12,"BYE")</f>
         <v>BYE</v>
       </c>
       <c r="C67" s="29"/>
@@ -7260,7 +7260,7 @@
     <row r="68" spans="1:20" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68" s="30"/>
       <c r="B68" s="47" t="str">
-        <f>IF(Voorronde!N13&gt;0,"["&amp;Voorronde!D13&amp;"] "&amp;Voorronde!E42,"BYE")</f>
+        <f>IF(Voorronde!N13&gt;0,"["&amp;Voorronde!D13&amp;"] "&amp;Voorronde!E13,"BYE")</f>
         <v>BYE</v>
       </c>
       <c r="C68" s="29"/>
@@ -7274,7 +7274,7 @@
     <row r="69" spans="1:20" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69" s="30"/>
       <c r="B69" s="47" t="str">
-        <f>IF(Voorronde!N14&gt;0,"["&amp;Voorronde!D14&amp;"] "&amp;Voorronde!E43,"BYE")</f>
+        <f>IF(Voorronde!N14&gt;0,"["&amp;Voorronde!D14&amp;"] "&amp;Voorronde!E14,"BYE")</f>
         <v>BYE</v>
       </c>
       <c r="C69" s="29"/>
@@ -7288,7 +7288,7 @@
     <row r="70" spans="1:20" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70" s="30"/>
       <c r="B70" s="47" t="str">
-        <f>IF(Voorronde!N15&gt;0,"["&amp;Voorronde!D15&amp;"] "&amp;Voorronde!E44,"BYE")</f>
+        <f>IF(Voorronde!N15&gt;0,"["&amp;Voorronde!D15&amp;"] "&amp;Voorronde!E15,"BYE")</f>
         <v>BYE</v>
       </c>
       <c r="C70" s="29"/>
@@ -7302,7 +7302,7 @@
     <row r="71" spans="1:20" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71" s="30"/>
       <c r="B71" s="47" t="str">
-        <f>IF(Voorronde!N16&gt;0,"["&amp;Voorronde!D16&amp;"] "&amp;Voorronde!E45,"BYE")</f>
+        <f>IF(Voorronde!N16&gt;0,"["&amp;Voorronde!D16&amp;"] "&amp;Voorronde!E16,"BYE")</f>
         <v>BYE</v>
       </c>
       <c r="C71" s="29"/>
@@ -7316,7 +7316,7 @@
     <row r="72" spans="1:20" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A72" s="30"/>
       <c r="B72" s="47" t="str">
-        <f>IF(Voorronde!N17&gt;0,"["&amp;Voorronde!D17&amp;"] "&amp;Voorronde!E46,"BYE")</f>
+        <f>IF(Voorronde!N17&gt;0,"["&amp;Voorronde!D17&amp;"] "&amp;Voorronde!E17,"BYE")</f>
         <v>BYE</v>
       </c>
       <c r="C72" s="29"/>
@@ -7326,7 +7326,7 @@
     <row r="73" spans="1:20" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A73" s="30"/>
       <c r="B73" s="47" t="str">
-        <f>IF(Voorronde!N18&gt;0,"["&amp;Voorronde!D18&amp;"] "&amp;Voorronde!E47,"BYE")</f>
+        <f>IF(Voorronde!N18&gt;0,"["&amp;Voorronde!D18&amp;"] "&amp;Voorronde!E18,"BYE")</f>
         <v>BYE</v>
       </c>
       <c r="C73" s="29"/>
@@ -7336,7 +7336,7 @@
     <row r="74" spans="1:20" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74" s="30"/>
       <c r="B74" s="47" t="str">
-        <f>IF(Voorronde!N19&gt;0,"["&amp;Voorronde!D19&amp;"] "&amp;Voorronde!E48,"BYE")</f>
+        <f>IF(Voorronde!N19&gt;0,"["&amp;Voorronde!D19&amp;"] "&amp;Voorronde!E19,"BYE")</f>
         <v>BYE</v>
       </c>
       <c r="C74" s="29"/>
@@ -7346,7 +7346,7 @@
     <row r="75" spans="1:20" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75" s="30"/>
       <c r="B75" s="47" t="str">
-        <f>IF(Voorronde!N20&gt;0,"["&amp;Voorronde!D20&amp;"] "&amp;Voorronde!E49,"BYE")</f>
+        <f>IF(Voorronde!N20&gt;0,"["&amp;Voorronde!D20&amp;"] "&amp;Voorronde!E20,"BYE")</f>
         <v>BYE</v>
       </c>
       <c r="C75" s="29"/>
@@ -7356,7 +7356,7 @@
     <row r="76" spans="1:20" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76" s="30"/>
       <c r="B76" s="47" t="str">
-        <f>IF(Voorronde!N21&gt;0,"["&amp;Voorronde!D21&amp;"] "&amp;Voorronde!E50,"BYE")</f>
+        <f>IF(Voorronde!N21&gt;0,"["&amp;Voorronde!D21&amp;"] "&amp;Voorronde!E21,"BYE")</f>
         <v>BYE</v>
       </c>
       <c r="C76" s="29"/>

</xml_diff>